<commit_message>
Opdatering af test materiale for import
</commit_message>
<xml_diff>
--- a/storage/app/public/test/import_test.xlsx
+++ b/storage/app/public/test/import_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92agg\Desktop\Svendeprøve\storage\app\public\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1273C8-B85C-4B41-B008-70BC3E1F488B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C4A6F4-AC1C-4744-A846-0AAE613F6CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-7260" windowWidth="16440" windowHeight="28320" xr2:uid="{577A64D8-9AE0-4645-8E34-BADD664AAAAB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>Title</t>
   </si>
@@ -111,6 +111,57 @@
   </si>
   <si>
     <t>import/Alina1.png</t>
+  </si>
+  <si>
+    <t>import/boerste-hindbaerbrus.png</t>
+  </si>
+  <si>
+    <t>Børste - hindbærbrus og røde nøjfer</t>
+  </si>
+  <si>
+    <t>”Forelskelse kan man ikke gardere sig imod. Her er man lovligt undskyldt ligesom under en stormflod!” siger fru Potersen, Børstes yndlingsnabo. ”Men kærlighed kan være strid, hvis den ikke bliver gengældt. Så sørg for at finde dig en kæreste, der ringer tilbage, Børste. Alt andet er spild af tid!”</t>
+  </si>
+  <si>
+    <t>Brugt</t>
+  </si>
+  <si>
+    <t>Ringenes Herre 1</t>
+  </si>
+  <si>
+    <t>Paperback-udgave med filmforside. Teksten er gennemrevideret af Jakob Levinsen, og alle appendikser er med. Derved udkommer værket for første gang på dansk i komplet version.Første bind af Tolkiens udødelige klassiker om hobbitten Frodo, der arver en mystisk ring af sin onkel Bilbo. Men Ringen tilhører den onde fyrst Sauron, der vil bruge</t>
+  </si>
+  <si>
+    <t>import/Ringenes-herre-1.png</t>
+  </si>
+  <si>
+    <t>Indbundet</t>
+  </si>
+  <si>
+    <t>Ringenes Herre 2</t>
+  </si>
+  <si>
+    <t>Paperback-udgave med filmforside. Teksten er gennemrevideret af Jakob Levinsen, og alle appendikser er med. Derved udkommer værket for første gang på dansk i komplet version.2. bind af Tolkiens udødelige klassiker om hobbitten Frodo</t>
+  </si>
+  <si>
+    <t>import/Ringenes-herre-2.png</t>
+  </si>
+  <si>
+    <t>import/Ringenes-herre-3.png</t>
+  </si>
+  <si>
+    <t>Ringenes Herre 3</t>
+  </si>
+  <si>
+    <t>Paperback-udgave med filmforside. Teksten er gennemrevideret af Jakob Levinsen, og alle appendikser er med. Derved udkommer værket for første gang på dansk i komplet version.3. bind af Tolkiens udødelige klassiker om hobbitten Frodo, der arver en mystisk ring af sin onkel Bilbo. Men Ringen tilhører den onde fyrst Sauron</t>
+  </si>
+  <si>
+    <t>Ringenes Herre og filosofien</t>
+  </si>
+  <si>
+    <t>Denne bog giver dig et indblik i filosofi i hobbithøjde. Ringenes Herre og filosofien forklarer filosofiske begreber og overvejelser med udgangspunkt i den populære kultserie fra J.R.R. Tolkien.</t>
+  </si>
+  <si>
+    <t>import/ringenes-herre-og-filosofien.png</t>
   </si>
 </sst>
 </file>
@@ -477,16 +528,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE0B03B4-E4AA-4CDF-9718-7F9FDC79B7D9}">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1"/>
     <col min="13" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -625,6 +679,226 @@
         <v>25</v>
       </c>
     </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>2145239867152</v>
+      </c>
+      <c r="D4" s="1">
+        <v>41141</v>
+      </c>
+      <c r="E4">
+        <v>131</v>
+      </c>
+      <c r="F4">
+        <v>221</v>
+      </c>
+      <c r="G4">
+        <v>140</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>9788702134575</v>
+      </c>
+      <c r="D5" s="1">
+        <v>41219</v>
+      </c>
+      <c r="E5">
+        <v>656</v>
+      </c>
+      <c r="F5">
+        <v>87</v>
+      </c>
+      <c r="G5">
+        <v>149</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>9788702134582</v>
+      </c>
+      <c r="D6" s="1">
+        <v>41219</v>
+      </c>
+      <c r="E6">
+        <v>544</v>
+      </c>
+      <c r="F6">
+        <v>81</v>
+      </c>
+      <c r="G6">
+        <v>249</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7">
+        <v>9788702134599</v>
+      </c>
+      <c r="D7" s="1">
+        <v>41219</v>
+      </c>
+      <c r="E7">
+        <v>644</v>
+      </c>
+      <c r="F7">
+        <v>72</v>
+      </c>
+      <c r="G7">
+        <v>169</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <v>9788772161433</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43815</v>
+      </c>
+      <c r="E8">
+        <v>295</v>
+      </c>
+      <c r="F8">
+        <v>41</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>